<commit_message>
Got Alt1 and Alt2 going
</commit_message>
<xml_diff>
--- a/CH-180 Hierarchical Structure.xlsx
+++ b/CH-180 Hierarchical Structure.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80FB03B-34DC-4FF2-8F7B-1D6EEC69D736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E697B65-6033-4F22-9576-33A35509C536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Alt1'!$E$2:$F$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt2'!$E$2:$F$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$E$2:$F$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +42,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="30">
   <si>
     <t>Result</t>
   </si>
@@ -135,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +203,12 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -290,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -320,6 +352,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -725,12 +761,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{619B2ED0-898E-44BA-9FD2-A3EA89F87A7F}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,4 +1024,708 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8817BCFB-E5CE-48A8-9C8D-B4A9D91074C1}">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" cm="1">
+        <f t="array" ref="B18:C29">_xlfn.LET(
+    _xlpm.a, B3:B13,
+    _xlpm.b, _xlfn.REDUCE(
+        {"A",1},
+        _xlfn.SEQUENCE(20),
+        _xlfn.LAMBDA(_xlpm.x,_xlpm.y,
+            _xlfn.VSTACK(
+                _xlpm.x,
+                _xlfn._xlws.FILTER(
+                    _xlfn.HSTACK(
+                        C3:C13,
+                        INDEX(_xlpm.x, _xlpm.y, 2) &amp; "-" &amp; _xlfn.MAP(_xlpm.a, _xlfn.LAMBDA(_xlpm.x, COUNTIF(B3:_xlpm.x, _xlpm.x)))
+                    ),
+                    _xlpm.a = INDEX(_xlpm.x, _xlpm.y, 1),
+                    ""
+                )
+            )
+        )
+    ),
+    _xlpm.c, _xlfn.TAKE(_xlpm.b, , 1),
+    _xlfn.HSTACK(_xlfn.TOCOL(_xlfn.TAKE(_xlpm.b, , -1), 3), _xlfn._xlws.FILTER(_xlpm.c, _xlpm.c &lt;&gt; ""))
+)</f>
+        <v>1</v>
+      </c>
+      <c r="C18" t="str">
+        <v>A</v>
+      </c>
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <v>1-1</v>
+      </c>
+      <c r="C19" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <v>1-2</v>
+      </c>
+      <c r="C20" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <v>1-3</v>
+      </c>
+      <c r="C21" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <v>1-1-1</v>
+      </c>
+      <c r="C22" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <v>1-1-2</v>
+      </c>
+      <c r="C23" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <v>1-2-1</v>
+      </c>
+      <c r="C24" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <v>1-1-1-1</v>
+      </c>
+      <c r="C25" t="str">
+        <v>G</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <v>1-2-1-1</v>
+      </c>
+      <c r="C26" t="str">
+        <v>M</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <v>1-2-1-2</v>
+      </c>
+      <c r="C27" t="str">
+        <v>N</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <v>1-2-1-2-1</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <v>1-2-1-2-1-1</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C828E012-039F-4BA3-9505-430F4C12731C}">
+  <dimension ref="A1:I36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="45.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="10"/>
+      <c r="I1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="11"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="str" cm="1">
+        <f t="array" ref="B19:C30">_xlfn.LET(
+    _xlpm.p, B3:B13,
+    _xlpm.c, C3:C13,
+    _xlfn.SORTBY(
+        _xlfn.REDUCE(
+            _xlfn.HSTACK(_xlfn.SINGLE(+_xlpm.p), "1"),
+            _xlpm.c,
+            _xlfn.LAMBDA(_xlpm.a,_xlpm.b,
+                _xlfn.LET(
+                    _xlpm.d, _xlfn.XLOOKUP(_xlpm.b, _xlpm.c, _xlpm.p),
+                    _xlfn.VSTACK(
+                        _xlpm.a,
+                        _xlfn.HSTACK(_xlpm.b, VLOOKUP(_xlpm.d, _xlpm.a, 2, ) &amp; -_xlfn.XMATCH(_xlpm.b, _xlfn._xlws.FILTER(_xlpm.c, _xlpm.p = _xlpm.d)))
+                    )
+                )
+            )
+        ),
+        {2,1}
+    )
+)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" t="str">
+        <v>A</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <v>1-1</v>
+      </c>
+      <c r="C20" t="str">
+        <v>B</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <v>1-2</v>
+      </c>
+      <c r="C21" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <v>1-3</v>
+      </c>
+      <c r="C22" t="str">
+        <v>D</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <v>1-1-1</v>
+      </c>
+      <c r="C23" t="str">
+        <v>E</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <v>1-1-2</v>
+      </c>
+      <c r="C24" t="str">
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <v>1-1-1-1</v>
+      </c>
+      <c r="C25" t="str">
+        <v>G</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <v>1-2-1</v>
+      </c>
+      <c r="C26" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <v>1-2-1-1</v>
+      </c>
+      <c r="C27" t="str">
+        <v>M</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <v>1-2-1-2</v>
+      </c>
+      <c r="C28" t="str">
+        <v>N</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <v>1-2-1-2-1</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Y</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <v>1-2-1-2-1-1</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Z</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>